<commit_message>
modified input behavior, implement Adhesion succes
</commit_message>
<xml_diff>
--- a/ra_exploer/examples/Adhesion_TR2_All.xlsx
+++ b/ra_exploer/examples/Adhesion_TR2_All.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\hp06316p\技術開發二處主管資料夾\缺智慧\Hobob\Summary\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="Adhesion_TR2_All" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -168,53 +163,51 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
+    <t>PI/Glass peeling</t>
+  </si>
+  <si>
+    <t>Seal/PI peeling</t>
+  </si>
+  <si>
+    <t>Seal/Seal peeling</t>
+  </si>
+  <si>
+    <t>十字法-雙PI-日產</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>十字法-雙PI-CMC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>T.B.D</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>Measure condition:
 Adhesion介面(T/C)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Measure condition:
 測試手法</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>PI/Glass peeling</t>
-  </si>
-  <si>
-    <t>Seal/PI peeling</t>
-  </si>
-  <si>
-    <t>Seal/Seal peeling</t>
-  </si>
-  <si>
-    <t>十字法-雙PI-日產</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>十字法-雙PI-CMC</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>T.B.D</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -222,21 +215,21 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -442,7 +435,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -477,7 +470,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -654,21 +647,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="14.25" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.375" style="4" bestFit="1" customWidth="1"/>
@@ -683,7 +676,7 @@
     <col min="11" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="31.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -700,10 +693,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>37</v>
@@ -715,7 +708,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="15" customFormat="1" ht="16.5">
       <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
@@ -747,7 +740,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="15" customFormat="1" ht="16.5">
       <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
@@ -779,7 +772,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="15" customFormat="1" ht="16.5">
       <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
@@ -811,7 +804,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="15" customFormat="1" ht="16.5">
       <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
@@ -843,7 +836,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="10" customFormat="1" ht="16.5">
       <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
@@ -875,7 +868,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="10" customFormat="1" ht="16.5">
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
@@ -907,7 +900,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="10" customFormat="1" ht="16.5">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
@@ -939,7 +932,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="10" customFormat="1" ht="16.5">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
@@ -971,7 +964,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="15" customFormat="1" ht="16.5">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
@@ -994,7 +987,7 @@
         <v>24</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I10" s="11" t="s">
         <v>25</v>
@@ -1003,7 +996,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="15" customFormat="1" ht="16.5">
       <c r="A11" s="11" t="s">
         <v>7</v>
       </c>
@@ -1026,7 +1019,7 @@
         <v>24</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I11" s="11" t="s">
         <v>25</v>
@@ -1035,7 +1028,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="15" customFormat="1" ht="16.5">
       <c r="A12" s="11" t="s">
         <v>7</v>
       </c>
@@ -1058,7 +1051,7 @@
         <v>24</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I12" s="11" t="s">
         <v>25</v>
@@ -1067,7 +1060,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="15" customFormat="1" ht="16.5">
       <c r="A13" s="11" t="s">
         <v>7</v>
       </c>
@@ -1090,7 +1083,7 @@
         <v>24</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I13" s="11" t="s">
         <v>25</v>
@@ -1099,7 +1092,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" s="15" customFormat="1" ht="16.5">
       <c r="A14" s="11" t="s">
         <v>7</v>
       </c>
@@ -1122,7 +1115,7 @@
         <v>24</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I14" s="11" t="s">
         <v>25</v>
@@ -1131,7 +1124,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="15" customFormat="1" ht="16.5">
       <c r="A15" s="11" t="s">
         <v>7</v>
       </c>
@@ -1154,7 +1147,7 @@
         <v>24</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I15" s="11" t="s">
         <v>25</v>
@@ -1163,7 +1156,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="10" customFormat="1">
       <c r="A16" s="6" t="s">
         <v>7</v>
       </c>
@@ -1183,7 +1176,7 @@
         <v>29</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H16" s="19" t="s">
         <v>30</v>
@@ -1195,7 +1188,7 @@
         <v>210416</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" s="10" customFormat="1">
       <c r="A17" s="6" t="s">
         <v>7</v>
       </c>
@@ -1215,7 +1208,7 @@
         <v>29</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H17" s="19" t="s">
         <v>32</v>
@@ -1227,7 +1220,7 @@
         <v>210416</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" s="10" customFormat="1">
       <c r="A18" s="6" t="s">
         <v>7</v>
       </c>
@@ -1247,7 +1240,7 @@
         <v>29</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H18" s="19" t="s">
         <v>30</v>
@@ -1259,7 +1252,7 @@
         <v>210416</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" s="10" customFormat="1">
       <c r="A19" s="6" t="s">
         <v>7</v>
       </c>
@@ -1279,7 +1272,7 @@
         <v>29</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H19" s="19" t="s">
         <v>32</v>
@@ -1291,7 +1284,7 @@
         <v>210416</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" s="10" customFormat="1">
       <c r="A20" s="6" t="s">
         <v>7</v>
       </c>
@@ -1311,7 +1304,7 @@
         <v>29</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H20" s="19" t="s">
         <v>30</v>
@@ -1323,7 +1316,7 @@
         <v>210416</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" s="10" customFormat="1">
       <c r="A21" s="6" t="s">
         <v>7</v>
       </c>
@@ -1343,7 +1336,7 @@
         <v>29</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H21" s="19" t="s">
         <v>32</v>
@@ -1355,7 +1348,7 @@
         <v>210416</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" s="10" customFormat="1">
       <c r="A22" s="6" t="s">
         <v>7</v>
       </c>
@@ -1375,7 +1368,7 @@
         <v>29</v>
       </c>
       <c r="G22" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H22" s="19" t="s">
         <v>30</v>
@@ -1387,7 +1380,7 @@
         <v>210416</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" s="10" customFormat="1">
       <c r="A23" s="6" t="s">
         <v>7</v>
       </c>
@@ -1407,7 +1400,7 @@
         <v>29</v>
       </c>
       <c r="G23" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H23" s="19" t="s">
         <v>32</v>
@@ -1419,7 +1412,7 @@
         <v>210416</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" s="15" customFormat="1">
       <c r="A24" s="11" t="s">
         <v>7</v>
       </c>
@@ -1439,10 +1432,10 @@
         <v>29</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I24" s="17" t="s">
         <v>35</v>
@@ -1451,7 +1444,7 @@
         <v>20201208</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" s="15" customFormat="1">
       <c r="A25" s="11" t="s">
         <v>7</v>
       </c>
@@ -1471,10 +1464,10 @@
         <v>29</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I25" s="17" t="s">
         <v>35</v>
@@ -1483,7 +1476,7 @@
         <v>20201208</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" s="15" customFormat="1">
       <c r="A26" s="11" t="s">
         <v>7</v>
       </c>
@@ -1503,10 +1496,10 @@
         <v>29</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I26" s="17" t="s">
         <v>35</v>
@@ -1515,7 +1508,7 @@
         <v>20201208</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" s="15" customFormat="1">
       <c r="A27" s="11" t="s">
         <v>7</v>
       </c>
@@ -1535,10 +1528,10 @@
         <v>29</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I27" s="17" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
modified test data and rm 'N.A' in configuration
</commit_message>
<xml_diff>
--- a/ra_exploer/examples/Adhesion_TR2_All.xlsx
+++ b/ra_exploer/examples/Adhesion_TR2_All.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\hp06316p\技術開發一部&amp;二部\技術開發一部\技術開發三課\個人暫存區\康良豪\RA選擇器\Summary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projects\td_toolkits_reconstruc\ra_exploer\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7965"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="19170" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="Adhesion_TR2_All" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="59">
   <si>
     <t>項目</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -183,10 +183,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>SNP07</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>7142T</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -211,10 +207,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>SNP07</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>2211, 膠寬 1000um</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -260,6 +252,10 @@
   </si>
   <si>
     <t>INX</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>S-NP07</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -824,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28:I34"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -880,13 +876,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E2" s="11">
         <v>0.8</v>
@@ -898,7 +894,7 @@
         <v>10</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I2" s="11" t="s">
         <v>11</v>
@@ -930,7 +926,7 @@
         <v>10</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>11</v>
@@ -962,7 +958,7 @@
         <v>10</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I4" s="11" t="s">
         <v>11</v>
@@ -994,7 +990,7 @@
         <v>10</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I5" s="11" t="s">
         <v>11</v>
@@ -1026,7 +1022,7 @@
         <v>15</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>16</v>
@@ -1058,7 +1054,7 @@
         <v>15</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>16</v>
@@ -1090,7 +1086,7 @@
         <v>15</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>16</v>
@@ -1122,7 +1118,7 @@
         <v>15</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>16</v>
@@ -1346,7 +1342,7 @@
         <v>33</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I16" s="19" t="s">
         <v>25</v>
@@ -1378,7 +1374,7 @@
         <v>33</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I17" s="19" t="s">
         <v>25</v>
@@ -1410,7 +1406,7 @@
         <v>33</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I18" s="19" t="s">
         <v>25</v>
@@ -1442,7 +1438,7 @@
         <v>33</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I19" s="19" t="s">
         <v>25</v>
@@ -1474,7 +1470,7 @@
         <v>33</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I20" s="19" t="s">
         <v>25</v>
@@ -1506,7 +1502,7 @@
         <v>33</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I21" s="19" t="s">
         <v>25</v>
@@ -1538,7 +1534,7 @@
         <v>33</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I22" s="19" t="s">
         <v>25</v>
@@ -1570,7 +1566,7 @@
         <v>33</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I23" s="19" t="s">
         <v>25</v>
@@ -1590,7 +1586,7 @@
         <v>8</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E24" s="17">
         <v>0.93</v>
@@ -1602,7 +1598,7 @@
         <v>34</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I24" s="17" t="s">
         <v>28</v>
@@ -1634,7 +1630,7 @@
         <v>34</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I25" s="17" t="s">
         <v>28</v>
@@ -1666,7 +1662,7 @@
         <v>34</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I26" s="17" t="s">
         <v>28</v>
@@ -1698,7 +1694,7 @@
         <v>34</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I27" s="17" t="s">
         <v>28</v>
@@ -1718,7 +1714,7 @@
         <v>38</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E28" s="22">
         <v>28.33</v>
@@ -1727,13 +1723,13 @@
         <v>24</v>
       </c>
       <c r="G28" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I28" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J28" s="22" t="s">
         <v>39</v>
@@ -1750,7 +1746,7 @@
         <v>38</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="E29" s="22">
         <v>29.67</v>
@@ -1759,13 +1755,13 @@
         <v>24</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I29" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J29" s="22" t="s">
         <v>39</v>
@@ -1782,7 +1778,7 @@
         <v>38</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E30" s="22">
         <v>32.75</v>
@@ -1791,30 +1787,30 @@
         <v>24</v>
       </c>
       <c r="G30" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I30" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J30" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="22" t="s">
+      <c r="D31" s="22" t="s">
         <v>44</v>
-      </c>
-      <c r="D31" s="22" t="s">
-        <v>45</v>
       </c>
       <c r="E31" s="22">
         <v>27.58</v>
@@ -1823,30 +1819,30 @@
         <v>24</v>
       </c>
       <c r="G31" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I31" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J31" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>29</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E32" s="22">
         <v>7.81</v>
@@ -1855,30 +1851,30 @@
         <v>24</v>
       </c>
       <c r="G32" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I32" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J32" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>29</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="E33" s="22">
         <v>18.760000000000002</v>
@@ -1887,30 +1883,30 @@
         <v>24</v>
       </c>
       <c r="G33" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I33" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J33" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>29</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E34" s="22">
         <v>13.23</v>
@@ -1919,16 +1915,16 @@
         <v>24</v>
       </c>
       <c r="G34" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I34" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J34" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>